<commit_message>
agrego data set file
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSetDesafioBootcamp.xlsx
+++ b/src/test/resources/DataSetDesafioBootcamp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bootcamp\DesafioBootcamp\FrameworkB15\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E620D56-5EAA-4C51-8BE5-50D94B904BC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C55F26-31F5-433B-A503-0F9BFF7F60F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,12 +17,23 @@
     <sheet name="Vuelos" sheetId="2" r:id="rId2"/>
     <sheet name="Trenes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>T</t>
   </si>
@@ -87,9 +98,6 @@
     <t>Email FormContact</t>
   </si>
   <si>
-    <t>Prefijo FormContact</t>
-  </si>
-  <si>
     <t>NroTel FormContact</t>
   </si>
   <si>
@@ -103,6 +111,33 @@
   </si>
   <si>
     <t>Montero</t>
+  </si>
+  <si>
+    <t>Introduce los 3 dígitos del código CVV de tu tarjeta.</t>
+  </si>
+  <si>
+    <t>Nro de credit card</t>
+  </si>
+  <si>
+    <t>4445 8889 4448 9999</t>
+  </si>
+  <si>
+    <t>enero</t>
+  </si>
+  <si>
+    <t>Mes credit card</t>
+  </si>
+  <si>
+    <t>Año credit card</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>NroPrefijo FormContact</t>
   </si>
 </sst>
 </file>
@@ -425,10 +460,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -444,7 +479,7 @@
     <col min="13" max="13" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1">
+    <row r="1" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -473,19 +508,31 @@
         <v>18</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>20</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>22</v>
+      <c r="N1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1">
+    <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -499,7 +546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1">
+    <row r="3" spans="1:17" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -515,7 +562,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1">
+    <row r="4" spans="1:17" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -523,7 +570,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="8">
         <v>25</v>
@@ -541,10 +588,10 @@
         <v>19</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" s="8">
         <v>54</v>
@@ -553,19 +600,82 @@
         <v>2.1312441455512301E+17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1">
+    <row r="5" spans="1:17" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="8">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="8">
+        <v>54</v>
+      </c>
+      <c r="M5" s="8">
+        <v>2494208260</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="8">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>4444</v>
+      </c>
     </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1">
+    <row r="6" spans="1:17" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="8">
+        <v>25</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1">
+    <row r="7" spans="1:17" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="8">
+        <v>25</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agrego data set al modulo de vuelos y dejo comentarios de posible solucion al TC-V04
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSetDesafioBootcamp.xlsx
+++ b/src/test/resources/DataSetDesafioBootcamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bootcamp\DesafioBootcamp\FrameworkB15\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C55F26-31F5-433B-A503-0F9BFF7F60F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A008F0A0-1DA6-4F06-BFC5-60F73B1E45D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hotel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>T</t>
   </si>
@@ -138,13 +138,73 @@
   </si>
   <si>
     <t>NroPrefijo FormContact</t>
+  </si>
+  <si>
+    <t>TC-V01</t>
+  </si>
+  <si>
+    <t>TC-V02</t>
+  </si>
+  <si>
+    <t>TC-V03</t>
+  </si>
+  <si>
+    <t>TC-V04</t>
+  </si>
+  <si>
+    <t>TC-V05</t>
+  </si>
+  <si>
+    <t>TC-V06</t>
+  </si>
+  <si>
+    <t>Buenos Aires (BUE)</t>
+  </si>
+  <si>
+    <t>Madrid (MAD)</t>
+  </si>
+  <si>
+    <t>American Express</t>
+  </si>
+  <si>
+    <t>Bebé, 0-11 meses</t>
+  </si>
+  <si>
+    <t>Asdasd</t>
+  </si>
+  <si>
+    <t>agustinvillanaon@gmail.com</t>
+  </si>
+  <si>
+    <t>eeeeee</t>
+  </si>
+  <si>
+    <t>rrrrrrrrrr</t>
+  </si>
+  <si>
+    <t>febrero</t>
+  </si>
+  <si>
+    <t>Avenida TSOFT</t>
+  </si>
+  <si>
+    <t>Madrid</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>Saavedra</t>
+  </si>
+  <si>
+    <t>agustinvilla5678@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -203,6 +263,16 @@
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -224,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -242,6 +312,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,9 +536,7 @@
   </sheetPr>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -689,13 +761,238 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
-  <sheetData/>
+  <cols>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="3">
+        <v>12</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="3">
+        <v>12</v>
+      </c>
+      <c r="F3" s="8">
+        <v>20</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="3">
+        <v>12</v>
+      </c>
+      <c r="F4" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="3">
+        <v>12</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6">
+        <v>54</v>
+      </c>
+      <c r="F6">
+        <v>1121856755</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" s="8">
+        <v>13</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1989</v>
+      </c>
+      <c r="M6" s="8">
+        <v>2</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="P6" s="8">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="8">
+        <v>1999</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="T6" s="8">
+        <v>1234</v>
+      </c>
+      <c r="U6" s="8">
+        <v>2234</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="X6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>25</v>
+      </c>
+      <c r="Z6" s="8">
+        <v>4444</v>
+      </c>
+      <c r="AA6" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="15.75" customHeight="1">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
+      </c>
+      <c r="C7">
+        <v>21</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="8">
+        <v>54</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1121856755</v>
+      </c>
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="L7" s="8">
+        <v>14</v>
+      </c>
+      <c r="M7" s="8">
+        <v>2000</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se actualizan case trenes
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSetDesafioBootcamp.xlsx
+++ b/src/test/resources/DataSetDesafioBootcamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Documents\BootCamp15_AcevedoGonzalo\ParteTecnica\FrameworkB15\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570287A3-ADCE-403B-8B68-797CD49A94AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053CE81A-ADFF-42F3-A699-96AF002202EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-78" yWindow="0" windowWidth="11676" windowHeight="13758" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hotel" sheetId="1" r:id="rId1"/>
@@ -1107,8 +1107,8 @@
   </sheetPr>
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1133,22 +1133,22 @@
         <v>13</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>66</v>
@@ -1203,23 +1203,23 @@
       <c r="E2">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="7">
+        <v>54</v>
+      </c>
+      <c r="J2" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K2">
         <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J2" s="7">
-        <v>54</v>
-      </c>
-      <c r="K2" s="7">
-        <v>4567879091</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>73</v>
@@ -1271,23 +1271,23 @@
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="7">
+        <v>54</v>
+      </c>
+      <c r="J3" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K3">
         <v>2</v>
-      </c>
-      <c r="G3" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="7">
-        <v>54</v>
-      </c>
-      <c r="K3" s="7">
-        <v>4567879091</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>73</v>
@@ -1339,12 +1339,12 @@
       <c r="E4">
         <v>5</v>
       </c>
-      <c r="F4">
+      <c r="H4" s="10"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
       <c r="L4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
@@ -1370,23 +1370,23 @@
       <c r="E5">
         <v>5</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="7">
+        <v>54</v>
+      </c>
+      <c r="J5" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K5">
         <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J5" s="7">
-        <v>54</v>
-      </c>
-      <c r="K5" s="7">
-        <v>4567879091</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>73</v>
@@ -1441,23 +1441,23 @@
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="7">
+        <v>54</v>
+      </c>
+      <c r="J6" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K6">
         <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J6" s="7">
-        <v>54</v>
-      </c>
-      <c r="K6" s="7">
-        <v>4567879091</v>
       </c>
       <c r="L6" s="7" t="s">
         <v>74</v>
@@ -1500,23 +1500,23 @@
       <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="7">
+        <v>54</v>
+      </c>
+      <c r="J7" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K7">
         <v>2</v>
-      </c>
-      <c r="G7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="7">
-        <v>54</v>
-      </c>
-      <c r="K7" s="7">
-        <v>4567879091</v>
       </c>
       <c r="L7" s="7" t="s">
         <v>73</v>
@@ -1546,8 +1546,8 @@
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{2FC8FD5C-7F55-41E7-A48F-B9C56DA6562C}"/>
-    <hyperlink ref="I3:I7" r:id="rId2" display="francisco.asis@gmail.com" xr:uid="{AB2E45BD-AFDF-40E5-839A-754AFF880DE4}"/>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{2FC8FD5C-7F55-41E7-A48F-B9C56DA6562C}"/>
+    <hyperlink ref="H3:H7" r:id="rId2" display="francisco.asis@gmail.com" xr:uid="{AB2E45BD-AFDF-40E5-839A-754AFF880DE4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Se actualiza data set trenes
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSetDesafioBootcamp.xlsx
+++ b/src/test/resources/DataSetDesafioBootcamp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Documents\BootCamp15_AcevedoGonzalo\ParteTecnica\FrameworkB15\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053CE81A-ADFF-42F3-A699-96AF002202EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4565E5DF-0D6D-447E-997E-12AD613EB2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4650" yWindow="3126" windowWidth="17280" windowHeight="9984" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hotel" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
   <si>
     <t>TittleOfCPs</t>
   </si>
@@ -1105,10 +1105,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:W7"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
@@ -1116,7 +1116,7 @@
     <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1181,13 +1181,16 @@
         <v>30</v>
       </c>
       <c r="V1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="X1" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" customHeight="1">
+    <row r="2" spans="1:24" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -1251,11 +1254,14 @@
       <c r="U2">
         <v>30</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="V2">
+        <v>345</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="15.75" customHeight="1">
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -1319,11 +1325,14 @@
       <c r="U3">
         <v>43</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="V3">
+        <v>345</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" customHeight="1">
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1352,9 +1361,9 @@
       <c r="R4" s="11"/>
       <c r="S4" s="12"/>
       <c r="T4" s="2"/>
-      <c r="V4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -1418,14 +1427,17 @@
       <c r="U5">
         <v>30</v>
       </c>
-      <c r="V5" s="2" t="s">
+      <c r="V5">
+        <v>345</v>
+      </c>
+      <c r="W5" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="W5" s="2" t="s">
+      <c r="X5" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:23" ht="15.75" customHeight="1">
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1482,9 +1494,9 @@
       </c>
       <c r="S6" s="12"/>
       <c r="T6" s="2"/>
-      <c r="V6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="15.75" customHeight="1">
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -1541,7 +1553,7 @@
       </c>
       <c r="S7" s="12"/>
       <c r="T7" s="2"/>
-      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="12" type="noConversion"/>

</xml_diff>

<commit_message>
arreglo data set, que se borro en un merge
</commit_message>
<xml_diff>
--- a/src/test/resources/DataSetDesafioBootcamp.xlsx
+++ b/src/test/resources/DataSetDesafioBootcamp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FrameworkB15\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gonzalo\Documents\BootCamp15_AcevedoGonzalo\ParteTecnica\FrameworkB15\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088AF020-F8AC-48F2-B773-EC2A50598BD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4565E5DF-0D6D-447E-997E-12AD613EB2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4650" yWindow="3126" windowWidth="17280" windowHeight="9984" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hotel" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
-  <si>
-    <t>T</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="82">
   <si>
     <t>TittleOfCPs</t>
   </si>
@@ -200,19 +197,88 @@
     <t>agustinvilla5678@gmail.com</t>
   </si>
   <si>
-    <t>Alicante (ALC)</t>
-  </si>
-  <si>
-    <t>Málaga (AGP)</t>
-  </si>
-  <si>
-    <t>"Esta es nuestra mejor oferta entre 789 opciones."</t>
-  </si>
-  <si>
-    <t>"Introduce el nombre."</t>
-  </si>
-  <si>
-    <t>El número de bebés (edad 0-1) no puede ser superior al de adultos.</t>
+    <t>Origen</t>
+  </si>
+  <si>
+    <t>Destino</t>
+  </si>
+  <si>
+    <t>Bilbao</t>
+  </si>
+  <si>
+    <t>TC-T01</t>
+  </si>
+  <si>
+    <t>TC-T02</t>
+  </si>
+  <si>
+    <t>TC-T03</t>
+  </si>
+  <si>
+    <t>TC-T04</t>
+  </si>
+  <si>
+    <t>TC-T05</t>
+  </si>
+  <si>
+    <t>TC-T06</t>
+  </si>
+  <si>
+    <t>Francisco</t>
+  </si>
+  <si>
+    <t>Asis</t>
+  </si>
+  <si>
+    <t>francisco.asis@gmail.com</t>
+  </si>
+  <si>
+    <t>Genero FormPassenger</t>
+  </si>
+  <si>
+    <t>Nombre FormPassenger</t>
+  </si>
+  <si>
+    <t>Apellido FormPassenger</t>
+  </si>
+  <si>
+    <t>Dia FormPassenger</t>
+  </si>
+  <si>
+    <t>Mes FormPassenger</t>
+  </si>
+  <si>
+    <t>Anio FormPassenger</t>
+  </si>
+  <si>
+    <t>Pasaporte FormPassenger</t>
+  </si>
+  <si>
+    <t>Sr</t>
+  </si>
+  <si>
+    <t>Sra</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Titular tarjeta</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>Fransico Asis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cupon Descuento </t>
+  </si>
+  <si>
+    <t>HOLIDAY100</t>
   </si>
 </sst>
 </file>
@@ -223,12 +289,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -289,16 +349,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color rgb="FF6AAB73"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -318,37 +385,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -567,200 +638,202 @@
   </sheetPr>
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="18.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="9" max="10" width="23.81640625" customWidth="1"/>
-    <col min="11" max="11" width="21.1796875" customWidth="1"/>
-    <col min="12" max="12" width="21.453125" customWidth="1"/>
-    <col min="13" max="13" width="31.26953125" customWidth="1"/>
+    <col min="9" max="10" width="23.83203125" customWidth="1"/>
+    <col min="11" max="11" width="21.1640625" customWidth="1"/>
+    <col min="12" max="12" width="21.44140625" customWidth="1"/>
+    <col min="13" max="13" width="31.27734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
+      <c r="D2" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>25</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="8">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="7">
         <v>25</v>
       </c>
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L4" s="7">
+        <v>54</v>
+      </c>
+      <c r="M4" s="7">
+        <v>2.1312441455512301E+17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" s="8">
-        <v>54</v>
-      </c>
-      <c r="M4" s="8">
-        <v>2.1312441455512301E+17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>25</v>
       </c>
       <c r="F5">
         <v>5</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="7">
+        <v>54</v>
+      </c>
+      <c r="M5" s="7">
+        <v>2494208260</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="O5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="P5" s="7">
         <v>25</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" s="8">
-        <v>54</v>
-      </c>
-      <c r="M5" s="8">
-        <v>2494208260</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="P5" s="8">
-        <v>25</v>
-      </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="7">
         <v>4444</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="8">
+      <c r="A6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="7">
         <v>25</v>
       </c>
       <c r="F6">
@@ -768,13 +841,13 @@
       </c>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A7" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="8">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="7">
         <v>25</v>
       </c>
       <c r="F7">
@@ -794,133 +867,121 @@
   </sheetPr>
   <dimension ref="A1:AA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="56.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.54296875" customWidth="1"/>
-    <col min="14" max="14" width="25.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>12</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" s="2">
+        <v>12</v>
+      </c>
+      <c r="F3" s="7">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="E3" s="3">
-        <v>12</v>
-      </c>
-      <c r="F3" s="8">
-        <v>20</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="12" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>56</v>
+        <v>36</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="3">
-        <v>28</v>
-      </c>
-      <c r="F4" s="8">
-        <v>7</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>57</v>
+        <v>42</v>
+      </c>
+      <c r="E4" s="2">
+        <v>12</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="D5" t="s">
         <v>42</v>
       </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>12</v>
       </c>
-      <c r="F5" s="8">
-        <v>22</v>
+      <c r="F5" s="7">
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H5">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" t="s">
         <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
       </c>
       <c r="E6">
         <v>54</v>
@@ -928,112 +989,109 @@
       <c r="F6">
         <v>1121856755</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>1</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="J6" s="8">
+      <c r="H6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="7">
         <v>13</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="L6" s="8">
+      <c r="K6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" s="7">
         <v>1989</v>
       </c>
-      <c r="M6" s="8">
+      <c r="M6" s="7">
         <v>2</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="O6" s="8" t="s">
+      <c r="P6" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="P6" s="8">
-        <v>14</v>
-      </c>
-      <c r="Q6" s="8" t="s">
+      <c r="R6" s="7">
+        <v>1999</v>
+      </c>
+      <c r="S6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="8">
-        <v>1999</v>
-      </c>
-      <c r="S6" s="8" t="s">
+      <c r="T6" s="7">
+        <v>1234</v>
+      </c>
+      <c r="U6" s="7">
+        <v>2234</v>
+      </c>
+      <c r="V6" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="T6" s="8">
-        <v>1234</v>
-      </c>
-      <c r="U6" s="8">
-        <v>2234</v>
-      </c>
-      <c r="V6" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="W6" s="8" t="s">
+      <c r="W6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="X6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="X6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y6" s="8">
+      <c r="Y6" s="7">
         <v>25</v>
       </c>
-      <c r="Z6" s="8">
+      <c r="Z6" s="7">
         <v>4444</v>
       </c>
-      <c r="AA6" s="8" t="s">
-        <v>26</v>
+      <c r="AA6" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>15</v>
       </c>
       <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="G7" s="7">
         <v>54</v>
       </c>
-      <c r="G7" s="8">
-        <v>54</v>
-      </c>
-      <c r="H7" s="8">
+      <c r="H7" s="7">
         <v>1121856755</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="9">
         <v>1</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>14</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="7">
         <v>2000</v>
-      </c>
-      <c r="N7" s="11" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1047,18 +1105,463 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.54296875" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="19" max="19" width="18.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:24" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" s="7">
+        <v>54</v>
+      </c>
+      <c r="J2" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" s="7">
+        <v>10</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>2000</v>
+      </c>
+      <c r="R2" s="11">
+        <v>39090453</v>
+      </c>
+      <c r="S2" s="12">
+        <v>4517629108566270</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="U2">
+        <v>30</v>
+      </c>
+      <c r="V2">
+        <v>345</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="7">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I3" s="7">
+        <v>54</v>
+      </c>
+      <c r="J3" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" t="s">
+        <v>64</v>
+      </c>
+      <c r="O3" s="7">
+        <v>10</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>2000</v>
+      </c>
+      <c r="R3" s="11">
+        <v>39090453</v>
+      </c>
+      <c r="S3" s="12">
+        <v>4517629108566270</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="U3">
+        <v>43</v>
+      </c>
+      <c r="V3">
+        <v>345</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="7">
+        <v>25</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="2"/>
+      <c r="W4" s="2"/>
+    </row>
+    <row r="5" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="7">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="7">
+        <v>54</v>
+      </c>
+      <c r="J5" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M5" t="s">
+        <v>63</v>
+      </c>
+      <c r="N5" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" s="7">
+        <v>10</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q5" s="7">
+        <v>2000</v>
+      </c>
+      <c r="R5" s="11">
+        <v>39090453</v>
+      </c>
+      <c r="S5" s="12">
+        <v>4517629108566270</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="U5">
+        <v>30</v>
+      </c>
+      <c r="V5">
+        <v>345</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X5" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="7">
+        <v>25</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I6" s="7">
+        <v>54</v>
+      </c>
+      <c r="J6" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" t="s">
+        <v>64</v>
+      </c>
+      <c r="O6" s="7">
+        <v>10</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q6" s="7">
+        <v>2014</v>
+      </c>
+      <c r="R6" s="11">
+        <v>39090453</v>
+      </c>
+      <c r="S6" s="12"/>
+      <c r="T6" s="2"/>
+      <c r="W6" s="2"/>
+    </row>
+    <row r="7" spans="1:24" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="7">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I7" s="7">
+        <v>54</v>
+      </c>
+      <c r="J7" s="7">
+        <v>4567879091</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="M7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N7" t="s">
+        <v>64</v>
+      </c>
+      <c r="O7" s="7">
+        <v>10</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q7" s="7">
+        <v>2023</v>
+      </c>
+      <c r="R7" s="11">
+        <v>39090453</v>
+      </c>
+      <c r="S7" s="12"/>
+      <c r="T7" s="2"/>
+      <c r="W7" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1" xr:uid="{2FC8FD5C-7F55-41E7-A48F-B9C56DA6562C}"/>
+    <hyperlink ref="H3:H7" r:id="rId2" display="francisco.asis@gmail.com" xr:uid="{AB2E45BD-AFDF-40E5-839A-754AFF880DE4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>